<commit_message>
content index is ready
</commit_message>
<xml_diff>
--- a/pandas_converted.xlsx
+++ b/pandas_converted.xlsx
@@ -16,61 +16,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
+    <t>ÁT</t>
+  </si>
+  <si>
+    <t>Rövid szöveg</t>
+  </si>
+  <si>
+    <t>Hosszú szöveg</t>
+  </si>
+  <si>
+    <t>TJ-menny.</t>
+  </si>
+  <si>
+    <t>VÁ-menny.</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Eá</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Óra</t>
+  </si>
+  <si>
+    <t>Anyag</t>
+  </si>
+  <si>
+    <t>Díj</t>
+  </si>
+  <si>
+    <t>15.</t>
+  </si>
+  <si>
+    <t>16.</t>
+  </si>
+  <si>
+    <t>17.</t>
+  </si>
+  <si>
+    <t>18.</t>
+  </si>
+  <si>
+    <t>Maradék</t>
+  </si>
+  <si>
+    <t>TÖ</t>
+  </si>
+  <si>
+    <t>FE.1</t>
+  </si>
+  <si>
     <t>TSZ</t>
-  </si>
-  <si>
-    <t>ÁT</t>
-  </si>
-  <si>
-    <t>Rövid szöveg</t>
-  </si>
-  <si>
-    <t>Hosszú szöveg</t>
-  </si>
-  <si>
-    <t>TJ-menny.</t>
-  </si>
-  <si>
-    <t>VÁ-menny.</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>Eá</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>Óra</t>
-  </si>
-  <si>
-    <t>Anyag</t>
-  </si>
-  <si>
-    <t>Díj</t>
-  </si>
-  <si>
-    <t>15.</t>
-  </si>
-  <si>
-    <t>16.</t>
-  </si>
-  <si>
-    <t>17.</t>
-  </si>
-  <si>
-    <t>18.</t>
-  </si>
-  <si>
-    <t>Maradék</t>
-  </si>
-  <si>
-    <t>TÖ</t>
-  </si>
-  <si>
-    <t>FE.1</t>
   </si>
   <si>
     <t>1</t>
@@ -580,13 +580,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,348 +644,279 @@
       <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
+      <c r="R2" t="s">
+        <v>67</v>
+      </c>
       <c r="S2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>42</v>
       </c>
+      <c r="R3" t="s">
+        <v>67</v>
+      </c>
       <c r="S3" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
         <v>42</v>
       </c>
+      <c r="R4" t="s">
+        <v>67</v>
+      </c>
       <c r="S4" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
         <v>43</v>
       </c>
+      <c r="R5" t="s">
+        <v>67</v>
+      </c>
       <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
         <v>44</v>
       </c>
+      <c r="R6" t="s">
+        <v>67</v>
+      </c>
       <c r="S6" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:19">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:19">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:19">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>48</v>
       </c>
+      <c r="R10" t="s">
+        <v>67</v>
+      </c>
       <c r="S10" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:19">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:19">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:19">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
+      <c r="R14" t="s">
+        <v>67</v>
+      </c>
       <c r="S14" t="s">
-        <v>67</v>
-      </c>
-      <c r="T14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:19">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:19">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:19">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
+      <c r="R18" t="s">
+        <v>67</v>
+      </c>
       <c r="S18" t="s">
-        <v>67</v>
-      </c>
-      <c r="T18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>57</v>
       </c>
+      <c r="R19" t="s">
+        <v>67</v>
+      </c>
       <c r="S19" t="s">
-        <v>67</v>
-      </c>
-      <c r="T19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>58</v>
       </c>
+      <c r="R20" t="s">
+        <v>67</v>
+      </c>
       <c r="S20" t="s">
-        <v>67</v>
-      </c>
-      <c r="T20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>58</v>
       </c>
+      <c r="R21" t="s">
+        <v>67</v>
+      </c>
       <c r="S21" t="s">
-        <v>67</v>
-      </c>
-      <c r="T21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
         <v>59</v>
       </c>
+      <c r="R22" t="s">
+        <v>67</v>
+      </c>
       <c r="S22" t="s">
-        <v>67</v>
-      </c>
-      <c r="T22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
         <v>60</v>
       </c>
+      <c r="R23" t="s">
+        <v>67</v>
+      </c>
       <c r="S23" t="s">
-        <v>67</v>
-      </c>
-      <c r="T23" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[fix] webapi convert more file endpoint
</commit_message>
<xml_diff>
--- a/pandas_converted.xlsx
+++ b/pandas_converted.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t>ÁT</t>
   </si>
@@ -97,18 +97,45 @@
     <t>02.01.0030.</t>
   </si>
   <si>
+    <t>02.01.0040.</t>
+  </si>
+  <si>
+    <t>02.01.0050.</t>
+  </si>
+  <si>
+    <t>02.01.0060.</t>
+  </si>
+  <si>
+    <t>02.01.0070.</t>
+  </si>
+  <si>
+    <t>02.01.0080.</t>
+  </si>
+  <si>
+    <t>02.01.0090.</t>
+  </si>
+  <si>
+    <t>02.01.0100.</t>
+  </si>
+  <si>
+    <t>02.01.0110.</t>
+  </si>
+  <si>
+    <t>02.01.0120.</t>
+  </si>
+  <si>
+    <t>02.01.0130.</t>
+  </si>
+  <si>
+    <t>02.01.0140.</t>
+  </si>
+  <si>
+    <t>02.01.0150.</t>
+  </si>
+  <si>
     <t>02.02.</t>
   </si>
   <si>
-    <t>02.02.0010.</t>
-  </si>
-  <si>
-    <t>02.02.0020.</t>
-  </si>
-  <si>
-    <t>02.02.0030.</t>
-  </si>
-  <si>
     <t>02.03.</t>
   </si>
   <si>
@@ -121,6 +148,42 @@
     <t>02.03.0030.</t>
   </si>
   <si>
+    <t>02.03.0040.</t>
+  </si>
+  <si>
+    <t>02.03.0050.</t>
+  </si>
+  <si>
+    <t>02.03.0060.</t>
+  </si>
+  <si>
+    <t>02.03.0070.</t>
+  </si>
+  <si>
+    <t>02.03.0080.</t>
+  </si>
+  <si>
+    <t>02.03.0090.</t>
+  </si>
+  <si>
+    <t>02.03.0100.</t>
+  </si>
+  <si>
+    <t>02.03.0110.</t>
+  </si>
+  <si>
+    <t>02.03.0120.</t>
+  </si>
+  <si>
+    <t>02.03.0130.</t>
+  </si>
+  <si>
+    <t>02.03.0140.</t>
+  </si>
+  <si>
+    <t>02.03.0150.</t>
+  </si>
+  <si>
     <t>03.</t>
   </si>
   <si>
@@ -151,41 +214,12 @@
     <t>Betonozás</t>
   </si>
   <si>
-    <t>Felső  talajréteg elszállítása engedéllyel rendelkező lerakóhelyre (e.i. 10 km távolság) (tömör m3)</t>
-  </si>
-  <si>
-    <t>Humusz terítése a területen 40 cm vastagságban</t>
-  </si>
-  <si>
-    <t>föld felrakás és elszállítás</t>
-  </si>
-  <si>
     <t>Zsaluzás</t>
   </si>
   <si>
-    <t>Ideiglenes talaj depónia kezelése</t>
-  </si>
-  <si>
-    <t>További bevágás termett talajba</t>
-  </si>
-  <si>
-    <t>Területelőkészítés összesen</t>
-  </si>
-  <si>
     <t>Betonacél</t>
   </si>
   <si>
-    <t>Feltöltés készítése csak I fázis
-100,90-től 102,10 mBf-ig 
-Töltés készítése 20/55 fagyálló murva beépítésével, rétegenkénti (rétegvastagság max 30 cm) tömörítéssel</t>
-  </si>
-  <si>
-    <t>Visszatöltés helyi anyagból</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Földmunkák </t>
-  </si>
-  <si>
     <t>Útépítés</t>
   </si>
   <si>
@@ -201,22 +235,134 @@
     <t>Vasúti pálya</t>
   </si>
   <si>
-    <t>28521</t>
-  </si>
-  <si>
-    <t>6893</t>
-  </si>
-  <si>
-    <t>2598</t>
-  </si>
-  <si>
-    <t>2706</t>
-  </si>
-  <si>
-    <t>53035</t>
-  </si>
-  <si>
-    <t>108</t>
+    <t>1900-01-02 00:00:00</t>
+  </si>
+  <si>
+    <t>1913-02-20 00:00:00</t>
+  </si>
+  <si>
+    <t>1900-01-30 00:00:00</t>
+  </si>
+  <si>
+    <t>1900-04-05 00:00:00</t>
+  </si>
+  <si>
+    <t>1900-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1901-08-22 00:00:00</t>
+  </si>
+  <si>
+    <t>Tápegység, akkumulátorral</t>
+  </si>
+  <si>
+    <t>R&amp;M</t>
+  </si>
+  <si>
+    <t>311</t>
+  </si>
+  <si>
+    <t>Ajánlatkészítés közben helyszíni bejárás, a helyszíni adottságok megismerése van lehetőség</t>
+  </si>
+  <si>
+    <t>1902-03-10 00:00:00</t>
+  </si>
+  <si>
+    <t>1909-11-08 00:00:00</t>
+  </si>
+  <si>
+    <t>1900-02-18 00:00:00</t>
+  </si>
+  <si>
+    <t>1900-01-03 00:00:00</t>
+  </si>
+  <si>
+    <t>Távnyitó licence</t>
+  </si>
+  <si>
+    <t>24portos LC duplex</t>
+  </si>
+  <si>
+    <t>8 as zónabővítő tápegységgel dobozzal akkumulátorral kompletten</t>
+  </si>
+  <si>
+    <t>A kivitelezés megkezdése előtt állapotrögzítés készítése az építésvezetés közreműködésével kötelező</t>
+  </si>
+  <si>
+    <t>10 db HSI 150-K/500 kábelátvezető rendszer elem vízszigetelt épületfalon kábeleátvezetéshez erős- és gyengeáramú rendszerek részére.</t>
+  </si>
+  <si>
+    <t>Merev szigetelő védőcső PVC-ből közepes mechanikai igénybevételre, szabadon vagy álmennyezet felett falon kívül szerelve, elágazó és szerelvény dobozokkal 
+Ø 25 mm</t>
+  </si>
+  <si>
+    <t>NYY-J kábel kábeltálcán, kábellétrán elhelyezve, vagy védőcsőbe húzva, 5x70 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L01 tervjelű lámpatest álmennyezetbe süllyesztetten szerelve.
+25 W, 3120 lm, 4000 K, LED fényforrással, IP20
+EAE BLOOM 3057188 BLM 025T 40OD00 3K1606020
+</t>
+  </si>
+  <si>
+    <t>1P kapcsoló süllyesztetten szerelve fehér színben, IP44</t>
+  </si>
+  <si>
+    <t>FE-U tervjelű szünetmentes hálózatú főelosztó berendezés</t>
+  </si>
+  <si>
+    <t>H07V-K szigetelt vezeték zöld/sárga szigetelés színnel EPH gerincvezeték céljára kábeltálcára fektetve, vagy védőcsőbe húzva, 
+16 mm2</t>
+  </si>
+  <si>
+    <t>1x12 OS2 kül-beltéri LSZH optikai kábel</t>
+  </si>
+  <si>
+    <t>PTZ kültéri kamera kerítés vonalban oszlopon elhelyezve</t>
+  </si>
+  <si>
+    <t>AWEX</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+During the preparation of the offer, it is recommended to visit the site and get to know the local conditions</t>
+  </si>
+  <si>
+    <t>Kábelárok készítése, 0,3 m szélességben, 0,8 m mélységben</t>
+  </si>
+  <si>
+    <t>Merev szigetelő védőcső PVC-ből közepes mechanikai igénybevételre, szabadon vagy álmennyezet felett falon kívül szerelve, elágazó és szerelvény dobozokkal 
+Ø 40 mm</t>
+  </si>
+  <si>
+    <t>NYY-J kábel kábeltálcán, kábellétrán elhelyezve, vagy védőcsőbe húzva, 5x50 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L02 tervjelű lámpatest álmennyezetbe süllyesztetten szerelve.
+38 W, 4493 lm, 4000 K, LED fényforrással, IP20
+EAE BLOOM 3072499 BLM 038T 40OD00 4K5606020
+</t>
+  </si>
+  <si>
+    <t>2P kapcsoló süllyesztetten szerelve fehér színben, IP44</t>
+  </si>
+  <si>
+    <t>E1N tervjelű normál hálózatú alelosztó berendezés</t>
+  </si>
+  <si>
+    <t>Ø 16 mm Horganyzott köracél (FeZn) felfogórúd betongúlában rögzítve, 1,5 m-es magassággal, villámvédelmi összekötő vezetékhez való csatlakozásnál csavaros kötőelemekkel, 100 kV-os szigetelő alátét lemezzel</t>
+  </si>
+  <si>
+    <t>Optikai patch panel</t>
+  </si>
+  <si>
+    <t>Végpont kamerák és rögzítők részére</t>
+  </si>
+  <si>
+    <t>Prior to the start of the construction, it is mandatory to make a condition record with the assistance of the construction management</t>
   </si>
   <si>
     <t>#REF!</t>
@@ -580,7 +726,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -650,13 +796,13 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -664,13 +810,13 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="R3" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="S3" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -678,13 +824,13 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="R4" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="S4" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -692,13 +838,13 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="S5" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -706,190 +852,160 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="R6" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="S6" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>46</v>
+      <c r="D8" t="s">
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>47</v>
+      <c r="D9" t="s">
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" t="s">
-        <v>67</v>
-      </c>
-      <c r="S10" t="s">
-        <v>68</v>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
-        <v>49</v>
+      <c r="D11" t="s">
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
-        <v>50</v>
+      <c r="D12" t="s">
+        <v>77</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>51</v>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14" t="s">
-        <v>67</v>
-      </c>
-      <c r="S14" t="s">
-        <v>68</v>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>65</v>
+      <c r="D15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>54</v>
+      <c r="D16" t="s">
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
-        <v>55</v>
+      <c r="E17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R18" t="s">
-        <v>67</v>
-      </c>
-      <c r="S18" t="s">
-        <v>68</v>
+      <c r="E18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="R19" t="s">
-        <v>67</v>
-      </c>
-      <c r="S19" t="s">
-        <v>68</v>
+      <c r="D19" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="R20" t="s">
-        <v>67</v>
-      </c>
-      <c r="S20" t="s">
-        <v>68</v>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="R21" t="s">
-        <v>67</v>
-      </c>
-      <c r="S21" t="s">
-        <v>68</v>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -897,13 +1013,13 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="R22" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="S22" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -911,13 +1027,244 @@
         <v>40</v>
       </c>
       <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="R23" t="s">
+        <v>113</v>
+      </c>
+      <c r="S23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="R39" t="s">
+        <v>113</v>
+      </c>
+      <c r="S39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" t="s">
+        <v>113</v>
+      </c>
+      <c r="S40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="R41" t="s">
+        <v>113</v>
+      </c>
+      <c r="S41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="R42" t="s">
+        <v>113</v>
+      </c>
+      <c r="S42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R23" t="s">
-        <v>67</v>
-      </c>
-      <c r="S23" t="s">
-        <v>68</v>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="R43" t="s">
+        <v>113</v>
+      </c>
+      <c r="S43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="R44" t="s">
+        <v>113</v>
+      </c>
+      <c r="S44" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>